<commit_message>
mysqli_stmt::bind_param(): Number of elements in type definition string doesn't match number of bind variables - Fix
</commit_message>
<xml_diff>
--- a/EzanaLMSData/XLSFiles/ezanaLMS_Students.xlsx
+++ b/EzanaLMSData/XLSFiles/ezanaLMS_Students.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="124">
   <si>
     <t xml:space="preserve">313c1c446d15cebc70fe2372980394160bc32c6c</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">1 Oct 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53c904468e7edec9a7f2501d8a8c8d5140c434cb</t>
   </si>
   <si>
     <t xml:space="preserve">324c1c446d15cebc70fe2372980394160bc32c6c</t>
@@ -398,11 +401,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -421,9 +425,15 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -468,7 +478,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -478,6 +488,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -498,19 +512,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.32"/>
@@ -557,31 +571,34 @@
       <c r="L1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>254737229776</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>900543292</v>
@@ -593,33 +610,36 @@
         <v>8</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>254737229777</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>900543293</v>
@@ -631,33 +651,36 @@
         <v>8</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>254737229778</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>900543294</v>
@@ -669,33 +692,36 @@
         <v>8</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>254737229779</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>900543295</v>
@@ -707,387 +733,420 @@
         <v>8</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>254737229780</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>900543296</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>254737229781</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>900543297</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>254737229782</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>900543298</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>254737229783</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>900543299</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>254737229784</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>900543300</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>254737229785</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>900543301</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>254737229786</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>900543302</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>254737229787</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>900543303</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K13" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>254737229788</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>900543304</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K14" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>254737229789</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>900543305</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K15" s="0" t="s">
         <v>8</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>